<commit_message>
enhanced the reporting added missing sheets
</commit_message>
<xml_diff>
--- a/workbook1.xlsx
+++ b/workbook1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProjects\ExcelFileCoparisionPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC564B37-F0D7-4674-9B74-4E340EAB86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D8B42-AB65-46A1-8328-B7B86DB845D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMP" sheetId="1" r:id="rId1"/>
-    <sheet name="DEPT" sheetId="2" r:id="rId2"/>
+    <sheet name="ExtraSheet" sheetId="3" r:id="rId2"/>
+    <sheet name="DEPT" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -438,7 +439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -778,6 +779,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4F0D46-83A9-4D5C-8876-8F4FD8B81ED6}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F889AC-8542-4FB7-9BE6-9669F6F45BD6}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>

<commit_message>
extracting the file name and handling floating values
</commit_message>
<xml_diff>
--- a/workbook1.xlsx
+++ b/workbook1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProjects\ExcelFileCoparisionPy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProjects\ExcelFileComparisionPy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049D8B42-AB65-46A1-8328-B7B86DB845D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BC85E6-A679-4051-9844-039DAFBC6B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMP" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>EMPNO</t>
   </si>
@@ -114,13 +114,26 @@
   </si>
   <si>
     <t>SALES</t>
+  </si>
+  <si>
+    <t>SHAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,10 +159,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,8 +171,12 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,8 +468,8 @@
     <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -497,10 +515,10 @@
       <c r="E2" s="2">
         <v>29572</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="3">
         <v>800</v>
       </c>
-      <c r="G2" s="1"/>
+      <c r="G2" s="3"/>
       <c r="H2" s="1">
         <v>20</v>
       </c>
@@ -521,10 +539,10 @@
       <c r="E3" s="2">
         <v>29637</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>1600</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>300</v>
       </c>
       <c r="H3" s="1">
@@ -547,10 +565,10 @@
       <c r="E4" s="2">
         <v>29639</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <v>1250</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="3">
         <v>500</v>
       </c>
       <c r="H4" s="1">
@@ -573,10 +591,10 @@
       <c r="E5" s="2">
         <v>29678</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <v>2975</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="3"/>
       <c r="H5" s="1">
         <v>20</v>
       </c>
@@ -597,10 +615,10 @@
       <c r="E6" s="2">
         <v>29707</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <v>2850</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="1">
         <v>30</v>
       </c>
@@ -621,10 +639,10 @@
       <c r="E7" s="2">
         <v>29746</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <v>2450</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="1">
         <v>10</v>
       </c>
@@ -645,10 +663,10 @@
       <c r="E8" s="2">
         <v>31886</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <v>3000</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="1">
         <v>20</v>
       </c>
@@ -667,10 +685,10 @@
       <c r="E9" s="2">
         <v>29907</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <v>5000</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="3"/>
       <c r="H9" s="1">
         <v>10</v>
       </c>
@@ -691,10 +709,10 @@
       <c r="E10" s="2">
         <v>29837</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="3">
         <v>1500</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>0</v>
       </c>
       <c r="H10" s="1">
@@ -717,10 +735,10 @@
       <c r="E11" s="2">
         <v>31920</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="3">
         <v>1100</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="1">
         <v>20</v>
       </c>
@@ -741,10 +759,10 @@
       <c r="E12" s="2">
         <v>29923</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="3">
         <v>950</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="1">
         <v>30</v>
       </c>
@@ -765,11 +783,35 @@
       <c r="E13" s="2">
         <v>29974</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="3">
         <v>1300</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>7936</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" s="1">
+        <v>7839</v>
+      </c>
+      <c r="E14" s="2">
+        <v>29974</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1300.9654</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1">
         <v>10</v>
       </c>
     </row>
@@ -782,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD4F0D46-83A9-4D5C-8876-8F4FD8B81ED6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>